<commit_message>
Revert "feat: add pytorch version of MLP and ALGO class"
This reverts commit 503ae91037cbe5f11442de39dadecacd565bc535, reversing
changes made to e0fc1191e931c742f83e1b3e67281a1fb2558549.
</commit_message>
<xml_diff>
--- a/trained_models/MLP/arrhythmia/results_table.xlsx
+++ b/trained_models/MLP/arrhythmia/results_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -475,152 +475,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>arrhythmia</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>(0, 1)</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>trained_models/MLP/arrhythmia/arrhythmia_(0, 1)_3_0</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>{'lr': 0.05, 'module__activation': 'tanh', 'module__dropout': 0.42213287429050866, 'module__topology': (278, 64, 32, 12), 'optimizer': &lt;class 'torch.optim.sgd.SGD'&gt;, 'optimizer__momentum': 0.3843817072926998, 'optimizer__nesterov': True}</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>0.5196850393700787</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>arrhythmia</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>(0, 1)</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>trained_models/MLP/arrhythmia/arrhythmia_(0, 1)_3_0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>{'lr': 0.05588135039273248, 'module__activation': 'tanh', 'module__dropout': 0.42213287429050866, 'module__topology': (278, 64, 32, 12), 'optimizer': &lt;class 'torch.optim.sgd.SGD'&gt;, 'optimizer__momentum': 0.3843817072926998, 'optimizer__nesterov': True}</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>0.5196850393700787</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>arrhythmia</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>(0, 1)</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>trained_models/MLP/arrhythmia/arrhythmia_(0, 1)_3_0</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'lr': 0.05588135039273248, 'module__activation': 'tanh', 'module__dropout': 0.42213287429050866, 'module__topology': (278, 64, 32, 12), 'optimizer': &lt;class 'torch.optim.sgd.SGD'&gt;, 'optimizer__momentum': 0.3843817072926998, 'optimizer__nesterov': True}</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>0.5196850393700787</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>arrhythmia</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>MLP</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>(0, 1)</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>trained_models/MLP/arrhythmia/arrhythmia_(0, 1)_3_0</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>{'lr': 0.04072567471680421, 'module__activation': 'tanh', 'module__dropout': 0.4923158114846535, 'module__topology': (278, 64, 12), 'optimizer': &lt;class 'torch.optim.sgd.SGD'&gt;, 'optimizer__momentum': 0.672041057147487, 'optimizer__nesterov': True}</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>0.6456692913385826</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>